<commit_message>
Add query where database was created and test queries of tables.
</commit_message>
<xml_diff>
--- a/DatabaseTables.xlsx
+++ b/DatabaseTables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Books Table</t>
   </si>
@@ -186,6 +186,39 @@
   </si>
   <si>
     <t>FK</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>nvarchar(60)</t>
+  </si>
+  <si>
+    <t>nvarchar(30)</t>
+  </si>
+  <si>
+    <t>nvarchar(25)</t>
+  </si>
+  <si>
+    <t>nvarchar(40)</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>nvarchar(10)</t>
+  </si>
+  <si>
+    <t>nchar(2)</t>
+  </si>
+  <si>
+    <t>nvarchar(20)</t>
+  </si>
+  <si>
+    <t>nchar(3)</t>
   </si>
 </sst>
 </file>
@@ -217,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -310,11 +343,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -329,6 +422,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -645,337 +755,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF77879-5F53-4FF7-8FF3-097AE319A345}">
-  <dimension ref="B2:O17"/>
+  <dimension ref="B2:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.7109375" customWidth="1"/>
-    <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="3" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="12" customWidth="1"/>
+    <col min="13" max="13" width="2.7109375" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" style="12" customWidth="1"/>
+    <col min="17" max="17" width="3" customWidth="1"/>
+    <col min="18" max="18" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:20" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="11"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="11"/>
+      <c r="J2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="K2" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="K2" s="21"/>
       <c r="L2" s="11"/>
       <c r="N2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="21"/>
+      <c r="P2" s="11"/>
+      <c r="R2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="11"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="S2" s="21"/>
+      <c r="T2" s="20"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="K3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="O3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="S3" s="18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T3" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="5"/>
       <c r="L4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="R4" s="6"/>
+      <c r="S4" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="T4" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="3" t="s">
+      <c r="H5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="4" t="s">
+      <c r="L5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="18" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="12"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="3" t="s">
+      <c r="H6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L6" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="K7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
+      <c r="D8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L8" t="s">
+      <c r="H8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="O8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="L9" t="s">
+      <c r="K9" s="21"/>
+      <c r="L9" s="11"/>
+      <c r="O9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="K10" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L10" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="K11" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L11" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="6"/>
+      <c r="K12" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L12" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="4" t="s">
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="D14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O14" s="21"/>
+      <c r="P14" s="11"/>
+    </row>
+    <row r="15" spans="2:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="11"/>
-      <c r="H15" s="10" t="s">
+      <c r="G15" s="22"/>
+      <c r="H15" s="20"/>
+      <c r="J15" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="11"/>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="21"/>
+      <c r="L15" s="11"/>
+      <c r="N15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="7" t="s">
+      <c r="O15" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="2" t="s">
+      <c r="P15" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="F16" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="G16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="K16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="6"/>
-      <c r="F17" s="4" t="s">
+      <c r="P16" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F17" s="16"/>
+      <c r="G17" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="4" t="s">
+      <c r="H17" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L17" s="4" t="s">
+      <c r="O17" s="18" t="s">
         <v>35</v>
+      </c>
+      <c r="P17" s="4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="R2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>